<commit_message>
Updated references and feature locations
</commit_message>
<xml_diff>
--- a/tabular/core/reference_feature_locations.xlsx
+++ b/tabular/core/reference_feature_locations.xlsx
@@ -1,29 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683E410D-6173-EF45-9DAC-D43C9C87642A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="26620" yWindow="1020" windowWidth="20860" windowHeight="24600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="90">
   <si>
     <t>featureName</t>
   </si>
@@ -148,9 +154,6 @@
     <t>SgCV</t>
   </si>
   <si>
-    <t xml:space="preserve">Cap </t>
-  </si>
-  <si>
     <t>Rep</t>
   </si>
   <si>
@@ -214,15 +217,6 @@
     <t>REF_SgCV</t>
   </si>
   <si>
-    <t>Orientation</t>
-  </si>
-  <si>
-    <t>(+)</t>
-  </si>
-  <si>
-    <t>(-)</t>
-  </si>
-  <si>
     <t>gp2</t>
   </si>
   <si>
@@ -247,18 +241,12 @@
     <t>ORF3</t>
   </si>
   <si>
-    <t>nonanuc</t>
-  </si>
-  <si>
     <t>NC_025683</t>
   </si>
   <si>
     <t>Po-Circo-like virus 41</t>
   </si>
   <si>
-    <t>Cap-rev</t>
-  </si>
-  <si>
     <t>Genus</t>
   </si>
   <si>
@@ -278,13 +266,46 @@
   </si>
   <si>
     <t>3UTR</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>ORFV2</t>
+  </si>
+  <si>
+    <t>ORFC2</t>
+  </si>
+  <si>
+    <t>gp3</t>
+  </si>
+  <si>
+    <t>AHEaCV-13</t>
+  </si>
+  <si>
+    <t>NC_026639</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>REF_AHEaCV-13</t>
+  </si>
+  <si>
+    <t>NC_026641</t>
+  </si>
+  <si>
+    <t>AHEaCV-14</t>
+  </si>
+  <si>
+    <t>REF_AHEaCV-14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,18 +349,15 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
     </font>
     <font>
       <sz val="10"/>
@@ -381,12 +399,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -409,6 +421,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2468,7 +2486,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2478,12 +2496,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2496,16 +2508,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2047">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -4890,38 +4903,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1505"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D8" sqref="A1:G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14" style="9" customWidth="1"/>
+    <col min="5" max="5" width="14" style="7" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
@@ -4932,25 +4944,22 @@
       <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="17" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>80</v>
+      <c r="C2" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -4958,415 +4967,367 @@
       <c r="G2" s="6">
         <v>54</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="17" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>80</v>
+      <c r="C3" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="6">
+        <v>55</v>
+      </c>
+      <c r="G3" s="6">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="6">
-        <v>2</v>
-      </c>
-      <c r="G3" s="6">
-        <v>10</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="17" t="s">
+      <c r="D4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="6">
+        <v>994</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="6">
-        <v>55</v>
-      </c>
-      <c r="G4" s="6">
-        <v>993</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="17" t="s">
+      <c r="C5" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1038</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="6">
-        <v>994</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1037</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>80</v>
+      <c r="C6" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6" s="6">
-        <v>1038</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1730</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>80</v>
+        <v>1731</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="F7" s="6">
-        <v>1731</v>
-      </c>
-      <c r="G7" s="19">
-        <v>1758</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>108</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>80</v>
+      <c r="C8" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F8" s="6">
-        <v>108</v>
+        <v>550</v>
       </c>
       <c r="G8" s="6">
-        <v>1007</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>80</v>
+      <c r="C9" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F9" s="6">
-        <v>550</v>
+        <v>1240</v>
       </c>
       <c r="G9" s="6">
-        <v>1026</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>80</v>
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>52</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F10" s="6">
-        <v>1240</v>
+        <v>32</v>
       </c>
       <c r="G10" s="6">
-        <v>1974</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="17" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>80</v>
+      <c r="C11" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="F11" s="6">
-        <v>32</v>
+        <v>1154</v>
       </c>
       <c r="G11" s="6">
-        <v>904</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>80</v>
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F12" s="6">
-        <v>1154</v>
+        <v>51</v>
       </c>
       <c r="G12" s="6">
-        <v>1906</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>80</v>
+      <c r="C13" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="F13" s="6">
-        <v>51</v>
+        <v>357</v>
       </c>
       <c r="G13" s="6">
-        <v>995</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>80</v>
+      <c r="C14" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F14" s="6">
-        <v>357</v>
+        <v>1034</v>
       </c>
       <c r="G14" s="6">
-        <v>671</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>80</v>
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F15" s="6">
-        <v>1034</v>
+        <v>48</v>
       </c>
       <c r="G15" s="6">
-        <v>1735</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="17" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>80</v>
+      <c r="C16" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F16" s="6">
-        <v>48</v>
+        <v>423</v>
       </c>
       <c r="G16" s="6">
-        <v>926</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="17" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>80</v>
+      <c r="C17" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F17" s="6">
-        <v>1212</v>
-      </c>
-      <c r="G17" s="6">
-        <v>1961</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="17" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G17" s="17">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>80</v>
+      <c r="C18" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="6">
         <v>37</v>
@@ -5374,25 +5335,22 @@
       <c r="G18" s="6">
         <v>906</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="17" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>80</v>
+      <c r="C19" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F19" s="6">
         <v>1190</v>
@@ -5400,25 +5358,22 @@
       <c r="G19" s="6">
         <v>2020</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="17" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>80</v>
+      <c r="C20" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="6">
         <v>36</v>
@@ -5426,25 +5381,22 @@
       <c r="G20" s="6">
         <v>911</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="17" t="s">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>80</v>
+      <c r="C21" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F21" s="6">
         <v>1116</v>
@@ -5452,25 +5404,22 @@
       <c r="G21" s="6">
         <v>1844</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="17" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>80</v>
+      <c r="C22" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="6">
         <v>100</v>
@@ -5478,1645 +5427,1700 @@
       <c r="G22" s="6">
         <v>1017</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="17" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>80</v>
+      <c r="C23" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F23" s="6">
+        <v>790</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="6">
         <v>1190</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G24" s="6">
         <v>1927</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="6">
-        <v>29</v>
-      </c>
-      <c r="G24" s="6">
-        <v>904</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>80</v>
+      <c r="C25" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F25" s="6">
+        <v>29</v>
+      </c>
+      <c r="G25" s="6">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="6">
         <v>614</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G26" s="6">
         <v>1063</v>
       </c>
-      <c r="H25" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="17" t="s">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B27" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="6">
+      <c r="C27" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="6">
         <v>48</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G27" s="6">
         <v>1007</v>
       </c>
-      <c r="H26" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="17" t="s">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B28" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="C28" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="6">
         <v>1261</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G28" s="6">
         <v>1761</v>
       </c>
-      <c r="H27" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="6">
-        <v>1</v>
-      </c>
-      <c r="G28" s="6">
-        <v>912</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>80</v>
+      <c r="C29" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F29" s="6">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="6">
         <v>1116</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G30" s="6">
         <v>1928</v>
       </c>
-      <c r="H29" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="6">
-        <v>36</v>
-      </c>
-      <c r="G30" s="6">
-        <v>929</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>80</v>
+      <c r="C31" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F31" s="6">
+        <v>36</v>
+      </c>
+      <c r="G31" s="6">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="6">
         <v>1020</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G32" s="6">
         <v>1703</v>
       </c>
-      <c r="H31" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="6">
-        <v>251</v>
-      </c>
-      <c r="G32" s="6">
-        <v>1195</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>80</v>
+      <c r="C33" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F33" s="6">
+        <v>251</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="6">
         <v>1251</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G34" s="6">
         <v>1934</v>
       </c>
-      <c r="H33" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="6">
-        <v>48</v>
-      </c>
-      <c r="G34" s="6">
-        <v>929</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>80</v>
+      <c r="C35" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F35" s="6">
+        <v>48</v>
+      </c>
+      <c r="G35" s="6">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="6">
         <v>968</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G36" s="6">
         <v>1723</v>
       </c>
-      <c r="H35" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="6">
-        <v>29</v>
-      </c>
-      <c r="G36" s="6">
-        <v>904</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="6">
+        <v>29</v>
+      </c>
+      <c r="G37" s="6">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="6">
-        <v>648</v>
-      </c>
-      <c r="G37" s="6">
-        <v>1400</v>
-      </c>
-      <c r="H37" s="8" t="s">
+      <c r="F38" s="6">
+        <v>1233</v>
+      </c>
+      <c r="G38" s="6">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="6">
+        <v>1289</v>
+      </c>
+      <c r="G39" s="6">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="6">
+        <v>1233</v>
+      </c>
+      <c r="G40" s="6">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" s="6">
+        <v>8</v>
+      </c>
+      <c r="G41" s="6">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="6">
+        <v>1055</v>
+      </c>
+      <c r="G42" s="6">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" s="6">
+        <v>216</v>
+      </c>
+      <c r="G43" s="6">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="6">
+        <v>1336</v>
+      </c>
+      <c r="G44" s="6">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="6">
-        <v>8</v>
-      </c>
-      <c r="G38" s="6">
-        <v>919</v>
-      </c>
-      <c r="H38" s="7" t="s">
+      <c r="C45" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="6">
+        <v>26</v>
+      </c>
+      <c r="G45" s="6">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" s="6">
+        <v>836</v>
+      </c>
+      <c r="G46" s="6">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F39" s="6">
-        <v>1055</v>
-      </c>
-      <c r="G39" s="6">
-        <v>1711</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="6">
-        <v>216</v>
-      </c>
-      <c r="G40" s="6">
-        <v>1106</v>
-      </c>
-      <c r="H40" s="7" t="s">
+      <c r="B47" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="6">
+        <v>208</v>
+      </c>
+      <c r="G47" s="6">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F41" s="6">
-        <v>1336</v>
-      </c>
-      <c r="G41" s="6">
-        <v>1980</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="13" t="s">
+      <c r="B48" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="F48" s="6">
+        <v>1005</v>
+      </c>
+      <c r="G48" s="6">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="C49" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="6">
-        <v>183</v>
-      </c>
-      <c r="G42" s="6">
-        <v>875</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="13" t="s">
+      <c r="F49" s="6">
+        <v>606</v>
+      </c>
+      <c r="G49" s="6">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="6">
+        <v>1741</v>
+      </c>
+      <c r="G50" s="6">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F51" s="6">
+        <v>2329</v>
+      </c>
+      <c r="G51" s="6">
+        <v>2904</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="6">
+        <v>68</v>
+      </c>
+      <c r="G52" s="6">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="6">
-        <v>855</v>
-      </c>
-      <c r="G43" s="6">
-        <v>1685</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="14" t="s">
+      <c r="F53" s="6">
+        <v>1164</v>
+      </c>
+      <c r="G53" s="6">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F54" s="6">
         <v>79</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="6">
-        <v>208</v>
-      </c>
-      <c r="G44" s="6">
-        <v>867</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="14" t="s">
+      <c r="G54" s="6">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F45" s="6">
-        <v>1005</v>
-      </c>
-      <c r="G45" s="6">
-        <v>1703</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F46" s="6">
-        <v>606</v>
-      </c>
-      <c r="G46" s="6">
-        <v>1583</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F47" s="6">
-        <v>1741</v>
-      </c>
-      <c r="G47" s="6">
-        <v>2313</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="6">
-        <v>2329</v>
-      </c>
-      <c r="G48" s="6">
-        <v>2904</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5">
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-    </row>
-    <row r="59" spans="2:5" ht="14" customHeight="1">
-      <c r="E59" s="10"/>
-    </row>
-    <row r="65" spans="2:5" ht="16" customHeight="1"/>
-    <row r="73" spans="2:5">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="11"/>
-    </row>
-    <row r="74" spans="2:5">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="11"/>
-    </row>
-    <row r="75" spans="2:5">
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="11"/>
-    </row>
-    <row r="76" spans="2:5">
+      <c r="F55" s="6">
+        <v>1139</v>
+      </c>
+      <c r="G55" s="6">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="8"/>
+    </row>
+    <row r="68" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="11"/>
-    </row>
-    <row r="77" spans="2:5">
+      <c r="E76" s="9"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="11"/>
-    </row>
-    <row r="78" spans="2:5">
+      <c r="E77" s="9"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="11"/>
-    </row>
-    <row r="79" spans="2:5">
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
-      <c r="E79" s="11"/>
-    </row>
-    <row r="80" spans="2:5">
+      <c r="E79" s="9"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
-      <c r="E80" s="11"/>
-    </row>
-    <row r="81" spans="2:7">
+      <c r="E80" s="9"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
-      <c r="E81" s="11"/>
-    </row>
-    <row r="82" spans="2:7">
+      <c r="E81" s="9"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
-      <c r="E82" s="11"/>
-      <c r="G82" s="2"/>
-    </row>
-    <row r="83" spans="2:7">
+      <c r="E82" s="9"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
-      <c r="E83" s="11"/>
-      <c r="G83" s="2"/>
-    </row>
-    <row r="84" spans="2:7">
+      <c r="E83" s="9"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
-      <c r="E84" s="11"/>
-    </row>
-    <row r="85" spans="2:7">
+      <c r="E84" s="9"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
-      <c r="E85" s="11"/>
-    </row>
-    <row r="86" spans="2:7">
+      <c r="E85" s="9"/>
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
-      <c r="E86" s="11"/>
-    </row>
-    <row r="87" spans="2:7">
+      <c r="E86" s="9"/>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
-      <c r="E87" s="11"/>
-    </row>
-    <row r="88" spans="2:7">
+      <c r="E87" s="9"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="11"/>
-    </row>
-    <row r="89" spans="2:7">
+      <c r="E88" s="9"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="11"/>
-    </row>
-    <row r="90" spans="2:7">
+      <c r="E89" s="9"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="11"/>
-    </row>
-    <row r="91" spans="2:7">
+      <c r="E90" s="9"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="11"/>
-    </row>
-    <row r="92" spans="2:7">
+      <c r="E91" s="9"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
-      <c r="E92" s="11"/>
-    </row>
-    <row r="93" spans="2:7">
+      <c r="E92" s="9"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
-      <c r="E93" s="11"/>
-    </row>
-    <row r="94" spans="2:7">
+      <c r="E93" s="9"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="11"/>
-    </row>
-    <row r="95" spans="2:7">
+      <c r="E94" s="9"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="11"/>
-    </row>
-    <row r="96" spans="2:7">
+      <c r="E95" s="9"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="11"/>
-    </row>
-    <row r="97" spans="2:6">
+      <c r="E96" s="9"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="11"/>
-    </row>
-    <row r="98" spans="2:6">
+      <c r="E97" s="9"/>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
-      <c r="E98" s="11"/>
-    </row>
-    <row r="99" spans="2:6">
+      <c r="E98" s="9"/>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="11"/>
-    </row>
-    <row r="100" spans="2:6">
+      <c r="E99" s="9"/>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
-      <c r="E100" s="11"/>
-    </row>
-    <row r="101" spans="2:6">
+      <c r="E100" s="9"/>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
-      <c r="E101" s="11"/>
-    </row>
-    <row r="102" spans="2:6">
+      <c r="E101" s="9"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
-      <c r="E102" s="11"/>
-    </row>
-    <row r="103" spans="2:6">
+      <c r="E102" s="9"/>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
-      <c r="E103" s="11"/>
-    </row>
-    <row r="104" spans="2:6">
+      <c r="E103" s="9"/>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="1"/>
-    </row>
-    <row r="105" spans="2:6">
+      <c r="E104" s="9"/>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
-      <c r="E105" s="11"/>
-    </row>
-    <row r="106" spans="2:6">
+      <c r="E105" s="9"/>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
-      <c r="E106" s="11"/>
-    </row>
-    <row r="107" spans="2:6">
+      <c r="E106" s="9"/>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
-      <c r="E107" s="11"/>
-    </row>
-    <row r="108" spans="2:6">
+      <c r="E107" s="9"/>
+      <c r="F107" s="1"/>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
-      <c r="E108" s="11"/>
-    </row>
-    <row r="109" spans="2:6">
+      <c r="E108" s="9"/>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
-    </row>
-    <row r="110" spans="2:6">
+      <c r="E109" s="9"/>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
-      <c r="E110" s="11"/>
-    </row>
-    <row r="111" spans="2:6">
+      <c r="E110" s="9"/>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
-      <c r="E111" s="11"/>
-    </row>
-    <row r="112" spans="2:6">
+      <c r="E111" s="9"/>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
-      <c r="E112" s="11"/>
-    </row>
-    <row r="113" spans="2:8">
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
-      <c r="E113" s="11"/>
-    </row>
-    <row r="114" spans="2:8">
+      <c r="E113" s="9"/>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
-      <c r="E114" s="11"/>
-    </row>
-    <row r="115" spans="2:8">
+      <c r="E114" s="9"/>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
-      <c r="E115" s="11"/>
-    </row>
-    <row r="116" spans="2:8">
+      <c r="E115" s="9"/>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
-      <c r="E116" s="11"/>
-    </row>
-    <row r="117" spans="2:8">
+      <c r="E116" s="9"/>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
-      <c r="E117" s="11"/>
-    </row>
-    <row r="118" spans="2:8">
+      <c r="E117" s="9"/>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
-      <c r="E118" s="11"/>
-      <c r="H118" s="2"/>
-    </row>
-    <row r="119" spans="2:8">
+      <c r="E118" s="9"/>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
-      <c r="E119" s="11"/>
-      <c r="H119" s="2"/>
-    </row>
-    <row r="120" spans="2:8">
+      <c r="E119" s="9"/>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
-      <c r="E120" s="11"/>
-      <c r="H120" s="2"/>
-    </row>
-    <row r="121" spans="2:8">
+      <c r="E120" s="9"/>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
-      <c r="E121" s="11"/>
-    </row>
-    <row r="122" spans="2:8">
+      <c r="E121" s="9"/>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
-      <c r="E122" s="11"/>
-    </row>
-    <row r="123" spans="2:8">
+      <c r="E122" s="9"/>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
-      <c r="E123" s="11"/>
-    </row>
-    <row r="124" spans="2:8">
+      <c r="E123" s="9"/>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
-      <c r="E124" s="11"/>
-    </row>
-    <row r="125" spans="2:8">
+      <c r="E124" s="9"/>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
-      <c r="E125" s="11"/>
-    </row>
-    <row r="126" spans="2:8">
+      <c r="E125" s="9"/>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
-      <c r="E126" s="11"/>
-    </row>
-    <row r="127" spans="2:8">
+      <c r="E126" s="9"/>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
-      <c r="E127" s="11"/>
-    </row>
-    <row r="128" spans="2:8">
+      <c r="E127" s="9"/>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
-      <c r="E128" s="11"/>
-    </row>
-    <row r="129" spans="2:5">
+      <c r="E128" s="9"/>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
-      <c r="E129" s="11"/>
-    </row>
-    <row r="130" spans="2:5">
+      <c r="E129" s="9"/>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
-      <c r="E130" s="11"/>
-    </row>
-    <row r="131" spans="2:5">
+      <c r="E130" s="9"/>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
-      <c r="E131" s="11"/>
-    </row>
-    <row r="132" spans="2:5">
+      <c r="E131" s="9"/>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="11"/>
-    </row>
-    <row r="133" spans="2:5">
+      <c r="E132" s="9"/>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="11"/>
-    </row>
-    <row r="134" spans="2:5">
+      <c r="E133" s="9"/>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="11"/>
-    </row>
-    <row r="135" spans="2:5">
+      <c r="E134" s="9"/>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="11"/>
-    </row>
-    <row r="136" spans="2:5">
+      <c r="E135" s="9"/>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
-      <c r="E136" s="11"/>
-    </row>
-    <row r="137" spans="2:5">
+      <c r="E136" s="9"/>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="11"/>
-    </row>
-    <row r="138" spans="2:5">
+      <c r="E137" s="9"/>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
-      <c r="E138" s="11"/>
-    </row>
-    <row r="139" spans="2:5">
+      <c r="E138" s="9"/>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
-      <c r="E139" s="11"/>
-    </row>
-    <row r="140" spans="2:5">
+      <c r="E139" s="9"/>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="11"/>
-    </row>
-    <row r="141" spans="2:5">
+      <c r="E140" s="9"/>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="11"/>
-    </row>
-    <row r="142" spans="2:5">
+      <c r="E141" s="9"/>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
-      <c r="E142" s="11"/>
-    </row>
-    <row r="143" spans="2:5">
+      <c r="E142" s="9"/>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="11"/>
-    </row>
-    <row r="144" spans="2:5">
+      <c r="E143" s="9"/>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
-      <c r="E144" s="11"/>
-    </row>
-    <row r="145" spans="2:5">
+      <c r="E144" s="9"/>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="11"/>
-    </row>
-    <row r="146" spans="2:5">
+      <c r="E145" s="9"/>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="11"/>
-    </row>
-    <row r="147" spans="2:5">
+      <c r="E146" s="9"/>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="11"/>
-    </row>
-    <row r="148" spans="2:5">
+      <c r="E147" s="9"/>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="11"/>
-    </row>
-    <row r="149" spans="2:5">
+      <c r="E148" s="9"/>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
-      <c r="E149" s="11"/>
-    </row>
-    <row r="150" spans="2:5">
+      <c r="E149" s="9"/>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
-      <c r="E150" s="11"/>
-    </row>
-    <row r="151" spans="2:5">
+      <c r="E150" s="9"/>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
-      <c r="E151" s="11"/>
-    </row>
-    <row r="169" spans="8:8">
-      <c r="H169" s="1"/>
-    </row>
-    <row r="170" spans="8:8">
-      <c r="H170" s="1"/>
-    </row>
-    <row r="171" spans="8:8">
-      <c r="H171" s="1"/>
-    </row>
-    <row r="172" spans="8:8">
-      <c r="H172" s="1"/>
-    </row>
-    <row r="173" spans="8:8">
-      <c r="H173" s="1"/>
-    </row>
-    <row r="174" spans="8:8">
-      <c r="H174" s="1"/>
-    </row>
-    <row r="227" spans="2:5">
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
-      <c r="D227" s="2"/>
-      <c r="E227" s="11"/>
-    </row>
-    <row r="228" spans="2:5">
-      <c r="B228" s="2"/>
-      <c r="C228" s="2"/>
-      <c r="D228" s="2"/>
-      <c r="E228" s="11"/>
-    </row>
-    <row r="229" spans="2:5">
-      <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
-      <c r="D229" s="2"/>
-      <c r="E229" s="11"/>
-    </row>
-    <row r="230" spans="2:5">
+      <c r="E151" s="9"/>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="9"/>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="9"/>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="9"/>
+    </row>
+    <row r="230" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
-      <c r="E230" s="11"/>
-    </row>
-    <row r="231" spans="2:5">
+      <c r="E230" s="9"/>
+    </row>
+    <row r="231" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
-      <c r="E231" s="11"/>
-    </row>
-    <row r="232" spans="2:5">
+      <c r="E231" s="9"/>
+    </row>
+    <row r="232" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
-      <c r="E232" s="11"/>
-    </row>
-    <row r="233" spans="2:5">
+      <c r="E232" s="9"/>
+    </row>
+    <row r="233" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
-      <c r="E233" s="11"/>
-    </row>
-    <row r="234" spans="2:5">
+      <c r="E233" s="9"/>
+    </row>
+    <row r="234" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
-      <c r="E234" s="11"/>
-    </row>
-    <row r="235" spans="2:5">
+      <c r="E234" s="9"/>
+    </row>
+    <row r="235" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
-      <c r="E235" s="11"/>
-    </row>
-    <row r="236" spans="2:5">
+      <c r="E235" s="9"/>
+    </row>
+    <row r="236" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
-      <c r="E236" s="11"/>
-    </row>
-    <row r="237" spans="2:5">
+      <c r="E236" s="9"/>
+    </row>
+    <row r="237" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
-      <c r="E237" s="11"/>
-    </row>
-    <row r="238" spans="2:5">
+      <c r="E237" s="9"/>
+    </row>
+    <row r="238" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
-      <c r="E238" s="11"/>
-    </row>
-    <row r="239" spans="2:5">
+      <c r="E238" s="9"/>
+    </row>
+    <row r="239" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
-      <c r="E239" s="11"/>
-    </row>
-    <row r="240" spans="2:5">
+      <c r="E239" s="9"/>
+    </row>
+    <row r="240" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
-      <c r="E240" s="11"/>
-    </row>
-    <row r="241" spans="2:5">
+      <c r="E240" s="9"/>
+    </row>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
-      <c r="E241" s="11"/>
-    </row>
-    <row r="242" spans="2:5">
+      <c r="E241" s="9"/>
+    </row>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
-      <c r="E242" s="11"/>
-    </row>
-    <row r="243" spans="2:5">
+      <c r="E242" s="9"/>
+    </row>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
-      <c r="E243" s="11"/>
-    </row>
-    <row r="244" spans="2:5">
+      <c r="E243" s="9"/>
+    </row>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
-      <c r="E244" s="11"/>
-    </row>
-    <row r="245" spans="2:5">
+      <c r="E244" s="9"/>
+    </row>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
-      <c r="E245" s="11"/>
-    </row>
-    <row r="246" spans="2:5">
+      <c r="E245" s="9"/>
+    </row>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
-      <c r="E246" s="11"/>
-    </row>
-    <row r="247" spans="2:5">
+      <c r="E246" s="9"/>
+    </row>
+    <row r="247" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
-      <c r="E247" s="11"/>
-    </row>
-    <row r="248" spans="2:5">
+      <c r="E247" s="9"/>
+    </row>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
-      <c r="E248" s="11"/>
-    </row>
-    <row r="249" spans="2:5">
+      <c r="E248" s="9"/>
+    </row>
+    <row r="249" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
-      <c r="E249" s="11"/>
-    </row>
-    <row r="250" spans="2:5">
+      <c r="E249" s="9"/>
+    </row>
+    <row r="250" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
-      <c r="E250" s="11"/>
-    </row>
-    <row r="251" spans="2:5">
+      <c r="E250" s="9"/>
+    </row>
+    <row r="251" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
-    </row>
-    <row r="252" spans="2:5">
+      <c r="E251" s="9"/>
+    </row>
+    <row r="252" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
-      <c r="E252" s="11"/>
-    </row>
-    <row r="253" spans="2:5">
+      <c r="E252" s="9"/>
+    </row>
+    <row r="253" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
-      <c r="E253" s="11"/>
-    </row>
-    <row r="254" spans="2:5">
+      <c r="E253" s="9"/>
+    </row>
+    <row r="254" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
-      <c r="E254" s="11"/>
-    </row>
-    <row r="255" spans="2:5">
+    </row>
+    <row r="255" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
-      <c r="E255" s="11"/>
-    </row>
-    <row r="256" spans="2:5">
+      <c r="E255" s="9"/>
+    </row>
+    <row r="256" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
-      <c r="E256" s="11"/>
-    </row>
-    <row r="257" spans="2:5">
+      <c r="E256" s="9"/>
+    </row>
+    <row r="257" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
-      <c r="E257" s="11"/>
-    </row>
-    <row r="258" spans="2:5">
+      <c r="E257" s="9"/>
+    </row>
+    <row r="258" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
-      <c r="E258" s="11"/>
-    </row>
-    <row r="941" spans="6:6">
-      <c r="F941" s="2"/>
-    </row>
-    <row r="1077" spans="2:4">
-      <c r="B1077" s="2"/>
-      <c r="C1077" s="2"/>
-      <c r="D1077" s="2"/>
-    </row>
-    <row r="1078" spans="2:4">
-      <c r="B1078" s="2"/>
-      <c r="C1078" s="2"/>
-      <c r="D1078" s="2"/>
-    </row>
-    <row r="1203" spans="2:4">
-      <c r="B1203" s="2"/>
-      <c r="C1203" s="2"/>
-      <c r="D1203" s="2"/>
-    </row>
-    <row r="1204" spans="2:4">
-      <c r="B1204" s="2"/>
-      <c r="C1204" s="2"/>
-      <c r="D1204" s="2"/>
-    </row>
-    <row r="1205" spans="2:4">
-      <c r="B1205" s="2"/>
-      <c r="C1205" s="2"/>
-      <c r="D1205" s="2"/>
-    </row>
-    <row r="1206" spans="2:4">
+      <c r="E258" s="9"/>
+    </row>
+    <row r="259" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B259" s="2"/>
+      <c r="C259" s="2"/>
+      <c r="D259" s="2"/>
+      <c r="E259" s="9"/>
+    </row>
+    <row r="260" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B260" s="2"/>
+      <c r="C260" s="2"/>
+      <c r="D260" s="2"/>
+      <c r="E260" s="9"/>
+    </row>
+    <row r="261" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B261" s="2"/>
+      <c r="C261" s="2"/>
+      <c r="D261" s="2"/>
+      <c r="E261" s="9"/>
+    </row>
+    <row r="944" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F944" s="2"/>
+    </row>
+    <row r="1080" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1080" s="2"/>
+      <c r="C1080" s="2"/>
+      <c r="D1080" s="2"/>
+    </row>
+    <row r="1081" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1081" s="2"/>
+      <c r="C1081" s="2"/>
+      <c r="D1081" s="2"/>
+    </row>
+    <row r="1206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1206" s="2"/>
       <c r="C1206" s="2"/>
       <c r="D1206" s="2"/>
     </row>
-    <row r="1207" spans="2:4">
+    <row r="1207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1207" s="2"/>
       <c r="C1207" s="2"/>
       <c r="D1207" s="2"/>
     </row>
-    <row r="1208" spans="2:4">
+    <row r="1208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1208" s="2"/>
       <c r="C1208" s="2"/>
       <c r="D1208" s="2"/>
     </row>
-    <row r="1253" spans="2:7">
-      <c r="F1253" s="2"/>
-      <c r="G1253" s="2"/>
-    </row>
-    <row r="1254" spans="2:7">
-      <c r="F1254" s="2"/>
-      <c r="G1254" s="2"/>
-    </row>
-    <row r="1255" spans="2:7">
-      <c r="F1255" s="2"/>
-      <c r="G1255" s="2"/>
-    </row>
-    <row r="1257" spans="2:7">
-      <c r="B1257" s="2"/>
-      <c r="C1257" s="2"/>
-      <c r="D1257" s="2"/>
-    </row>
-    <row r="1258" spans="2:7">
-      <c r="B1258" s="2"/>
-      <c r="C1258" s="2"/>
-      <c r="D1258" s="2"/>
-    </row>
-    <row r="1259" spans="2:7">
-      <c r="B1259" s="2"/>
-      <c r="C1259" s="2"/>
-      <c r="D1259" s="2"/>
-    </row>
-    <row r="1260" spans="2:7">
+    <row r="1209" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1209" s="2"/>
+      <c r="C1209" s="2"/>
+      <c r="D1209" s="2"/>
+    </row>
+    <row r="1210" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1210" s="2"/>
+      <c r="C1210" s="2"/>
+      <c r="D1210" s="2"/>
+    </row>
+    <row r="1211" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1211" s="2"/>
+      <c r="C1211" s="2"/>
+      <c r="D1211" s="2"/>
+    </row>
+    <row r="1256" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F1256" s="2"/>
+      <c r="G1256" s="2"/>
+    </row>
+    <row r="1257" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F1257" s="2"/>
+      <c r="G1257" s="2"/>
+    </row>
+    <row r="1258" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F1258" s="2"/>
+      <c r="G1258" s="2"/>
+    </row>
+    <row r="1260" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1260" s="2"/>
       <c r="C1260" s="2"/>
       <c r="D1260" s="2"/>
     </row>
-    <row r="1261" spans="2:7">
+    <row r="1261" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1261" s="2"/>
       <c r="C1261" s="2"/>
       <c r="D1261" s="2"/>
     </row>
-    <row r="1280" spans="2:4">
-      <c r="B1280" s="2"/>
-      <c r="C1280" s="2"/>
-      <c r="D1280" s="2"/>
-    </row>
-    <row r="1281" spans="2:4">
-      <c r="B1281" s="2"/>
-      <c r="C1281" s="2"/>
-      <c r="D1281" s="2"/>
-    </row>
-    <row r="1282" spans="2:4">
-      <c r="B1282" s="2"/>
-      <c r="C1282" s="2"/>
-      <c r="D1282" s="2"/>
-    </row>
-    <row r="1283" spans="2:4">
+    <row r="1262" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1262" s="2"/>
+      <c r="C1262" s="2"/>
+      <c r="D1262" s="2"/>
+    </row>
+    <row r="1263" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1263" s="2"/>
+      <c r="C1263" s="2"/>
+      <c r="D1263" s="2"/>
+    </row>
+    <row r="1264" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1264" s="2"/>
+      <c r="C1264" s="2"/>
+      <c r="D1264" s="2"/>
+    </row>
+    <row r="1283" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1283" s="2"/>
       <c r="C1283" s="2"/>
       <c r="D1283" s="2"/>
     </row>
-    <row r="1284" spans="2:4">
+    <row r="1284" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1284" s="2"/>
       <c r="C1284" s="2"/>
       <c r="D1284" s="2"/>
     </row>
-    <row r="1285" spans="2:4">
+    <row r="1285" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1285" s="2"/>
       <c r="C1285" s="2"/>
       <c r="D1285" s="2"/>
     </row>
-    <row r="1286" spans="2:4">
+    <row r="1286" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1286" s="2"/>
       <c r="C1286" s="2"/>
       <c r="D1286" s="2"/>
     </row>
-    <row r="1288" spans="2:4">
+    <row r="1287" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1287" s="2"/>
+      <c r="C1287" s="2"/>
+      <c r="D1287" s="2"/>
+    </row>
+    <row r="1288" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1288" s="2"/>
       <c r="C1288" s="2"/>
       <c r="D1288" s="2"/>
     </row>
-    <row r="1289" spans="2:4">
+    <row r="1289" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1289" s="2"/>
       <c r="C1289" s="2"/>
       <c r="D1289" s="2"/>
     </row>
-    <row r="1290" spans="2:4">
-      <c r="B1290" s="2"/>
-      <c r="C1290" s="2"/>
-      <c r="D1290" s="2"/>
-    </row>
-    <row r="1291" spans="2:4">
+    <row r="1291" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1291" s="2"/>
       <c r="C1291" s="2"/>
       <c r="D1291" s="2"/>
     </row>
-    <row r="1292" spans="2:4">
+    <row r="1292" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1292" s="2"/>
       <c r="C1292" s="2"/>
       <c r="D1292" s="2"/>
     </row>
-    <row r="1293" spans="2:4">
+    <row r="1293" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1293" s="2"/>
       <c r="C1293" s="2"/>
       <c r="D1293" s="2"/>
     </row>
-    <row r="1345" spans="2:4">
-      <c r="B1345" s="2"/>
-      <c r="C1345" s="2"/>
-      <c r="D1345" s="2"/>
-    </row>
-    <row r="1346" spans="2:4">
-      <c r="B1346" s="2"/>
-      <c r="C1346" s="2"/>
-      <c r="D1346" s="2"/>
-    </row>
-    <row r="1347" spans="2:4">
-      <c r="B1347" s="2"/>
-      <c r="C1347" s="2"/>
-      <c r="D1347" s="2"/>
-    </row>
-    <row r="1348" spans="2:4">
+    <row r="1294" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1294" s="2"/>
+      <c r="C1294" s="2"/>
+      <c r="D1294" s="2"/>
+    </row>
+    <row r="1295" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1295" s="2"/>
+      <c r="C1295" s="2"/>
+      <c r="D1295" s="2"/>
+    </row>
+    <row r="1296" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1296" s="2"/>
+      <c r="C1296" s="2"/>
+      <c r="D1296" s="2"/>
+    </row>
+    <row r="1348" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1348" s="2"/>
       <c r="C1348" s="2"/>
       <c r="D1348" s="2"/>
     </row>
-    <row r="1350" spans="2:4">
+    <row r="1349" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1349" s="2"/>
+      <c r="C1349" s="2"/>
+      <c r="D1349" s="2"/>
+    </row>
+    <row r="1350" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1350" s="2"/>
       <c r="C1350" s="2"/>
       <c r="D1350" s="2"/>
     </row>
-    <row r="1351" spans="2:4">
+    <row r="1351" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1351" s="2"/>
       <c r="C1351" s="2"/>
       <c r="D1351" s="2"/>
     </row>
-    <row r="1352" spans="2:4">
-      <c r="B1352" s="2"/>
-      <c r="C1352" s="2"/>
-      <c r="D1352" s="2"/>
-    </row>
-    <row r="1353" spans="2:4">
+    <row r="1353" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1353" s="2"/>
       <c r="C1353" s="2"/>
       <c r="D1353" s="2"/>
     </row>
-    <row r="1388" spans="2:4">
-      <c r="B1388" s="2"/>
-      <c r="C1388" s="2"/>
-      <c r="D1388" s="2"/>
-    </row>
-    <row r="1389" spans="2:4">
-      <c r="B1389" s="2"/>
-      <c r="C1389" s="2"/>
-      <c r="D1389" s="2"/>
-    </row>
-    <row r="1390" spans="2:4">
-      <c r="B1390" s="2"/>
-      <c r="C1390" s="2"/>
-      <c r="D1390" s="2"/>
-    </row>
-    <row r="1391" spans="2:4">
+    <row r="1354" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1354" s="2"/>
+      <c r="C1354" s="2"/>
+      <c r="D1354" s="2"/>
+    </row>
+    <row r="1355" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1355" s="2"/>
+      <c r="C1355" s="2"/>
+      <c r="D1355" s="2"/>
+    </row>
+    <row r="1356" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1356" s="2"/>
+      <c r="C1356" s="2"/>
+      <c r="D1356" s="2"/>
+    </row>
+    <row r="1391" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1391" s="2"/>
       <c r="C1391" s="2"/>
       <c r="D1391" s="2"/>
     </row>
-    <row r="1392" spans="2:4">
+    <row r="1392" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1392" s="2"/>
       <c r="C1392" s="2"/>
       <c r="D1392" s="2"/>
     </row>
-    <row r="1393" spans="2:4">
+    <row r="1393" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1393" s="2"/>
       <c r="C1393" s="2"/>
       <c r="D1393" s="2"/>
     </row>
-    <row r="1435" spans="5:7">
-      <c r="F1435" s="2"/>
-      <c r="G1435" s="2"/>
-    </row>
-    <row r="1436" spans="5:7">
-      <c r="E1436" s="12"/>
-      <c r="F1436" s="2"/>
-      <c r="G1436" s="2"/>
-    </row>
-    <row r="1437" spans="5:7">
-      <c r="E1437" s="12"/>
-      <c r="F1437" s="2"/>
-      <c r="G1437" s="2"/>
-    </row>
-    <row r="1438" spans="5:7">
-      <c r="E1438" s="12"/>
+    <row r="1394" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1394" s="2"/>
+      <c r="C1394" s="2"/>
+      <c r="D1394" s="2"/>
+    </row>
+    <row r="1395" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1395" s="2"/>
+      <c r="C1395" s="2"/>
+      <c r="D1395" s="2"/>
+    </row>
+    <row r="1396" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1396" s="2"/>
+      <c r="C1396" s="2"/>
+      <c r="D1396" s="2"/>
+    </row>
+    <row r="1438" spans="5:7" x14ac:dyDescent="0.2">
       <c r="F1438" s="2"/>
       <c r="G1438" s="2"/>
     </row>
-    <row r="1439" spans="5:7">
+    <row r="1439" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1439" s="10"/>
       <c r="F1439" s="2"/>
       <c r="G1439" s="2"/>
     </row>
-    <row r="1502" spans="2:4">
-      <c r="B1502" s="2"/>
-      <c r="C1502" s="2"/>
-      <c r="D1502" s="2"/>
-    </row>
-    <row r="1503" spans="2:4">
-      <c r="B1503" s="2"/>
-      <c r="C1503" s="2"/>
-      <c r="D1503" s="2"/>
-    </row>
-    <row r="1504" spans="2:4">
-      <c r="B1504" s="2"/>
-      <c r="C1504" s="2"/>
-      <c r="D1504" s="2"/>
-    </row>
-    <row r="1505" spans="2:4">
+    <row r="1440" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1440" s="10"/>
+      <c r="F1440" s="2"/>
+      <c r="G1440" s="2"/>
+    </row>
+    <row r="1441" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1441" s="10"/>
+      <c r="F1441" s="2"/>
+      <c r="G1441" s="2"/>
+    </row>
+    <row r="1442" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F1442" s="2"/>
+      <c r="G1442" s="2"/>
+    </row>
+    <row r="1505" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1505" s="2"/>
       <c r="C1505" s="2"/>
       <c r="D1505" s="2"/>
     </row>
+    <row r="1506" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1506" s="2"/>
+      <c r="C1506" s="2"/>
+      <c r="D1506" s="2"/>
+    </row>
+    <row r="1507" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1507" s="2"/>
+      <c r="C1507" s="2"/>
+      <c r="D1507" s="2"/>
+    </row>
+    <row r="1508" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1508" s="2"/>
+      <c r="C1508" s="2"/>
+      <c r="D1508" s="2"/>
+    </row>
   </sheetData>
-  <sortState ref="A3:H48">
-    <sortCondition ref="C3:C48"/>
-    <sortCondition ref="A3:A48"/>
-    <sortCondition ref="F3:F48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G51">
+    <sortCondition ref="C3:C51"/>
+    <sortCondition ref="A3:A51"/>
+    <sortCondition ref="F3:F51"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7129,16 +7133,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -7152,7 +7156,7 @@
         <v>2920</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7166,7 +7170,7 @@
         <v>3302</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added new reference sequences
</commit_message>
<xml_diff>
--- a/tabular/core/reference_feature_locations.xlsx
+++ b/tabular/core/reference_feature_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D270D2CD-B94C-4B42-A8C8-62A76A9FB761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FC644A-BE4E-8843-B39B-16BBD8C9AE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26620" yWindow="1020" windowWidth="20860" windowHeight="24600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="96">
   <si>
     <t>featureName</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>CoCV</t>
+  </si>
+  <si>
+    <t>REF_FlCyV</t>
+  </si>
+  <si>
+    <t>NC_024700</t>
+  </si>
+  <si>
+    <t>Feline cyclovirus</t>
   </si>
 </sst>
 </file>
@@ -4913,10 +4922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1511"/>
+  <dimension ref="A1:G1513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B34" sqref="A1:G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6174,113 +6183,147 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>85</v>
+      <c r="A55" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>41</v>
       </c>
       <c r="F55" s="6">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="G55" s="6">
-        <v>1171</v>
+        <v>819</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>85</v>
+      <c r="A56" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>79</v>
       </c>
       <c r="F56" s="6">
-        <v>1164</v>
+        <v>827</v>
       </c>
       <c r="G56" s="6">
-        <v>2060</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>87</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>88</v>
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>85</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>41</v>
       </c>
       <c r="F57" s="6">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G57" s="6">
-        <v>1149</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" t="s">
-        <v>88</v>
+      <c r="A58" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="C58" s="19" t="s">
         <v>85</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>79</v>
       </c>
       <c r="F58" s="6">
+        <v>1164</v>
+      </c>
+      <c r="G58" s="6">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F59" s="6">
+        <v>79</v>
+      </c>
+      <c r="G59" s="6">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F60" s="6">
         <v>1139</v>
       </c>
-      <c r="G58" s="6">
+      <c r="G60" s="6">
         <v>2086</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E65" s="8"/>
-    </row>
-    <row r="71" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="9"/>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="9"/>
-    </row>
+    <row r="67" spans="5:5" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="8"/>
+    </row>
+    <row r="73" spans="5:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -6328,26 +6371,26 @@
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="9"/>
-      <c r="G88" s="2"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="9"/>
-      <c r="G89" s="2"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="9"/>
+      <c r="G90" s="2"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="9"/>
+      <c r="G91" s="2"/>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B92" s="2"/>
@@ -6462,7 +6505,6 @@
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="9"/>
-      <c r="F110" s="1"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B111" s="2"/>
@@ -6475,6 +6517,7 @@
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
       <c r="E112" s="9"/>
+      <c r="F112" s="1"/>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B113" s="2"/>
@@ -6492,6 +6535,7 @@
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
+      <c r="E115" s="9"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
@@ -6503,7 +6547,6 @@
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
-      <c r="E117" s="9"/>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B118" s="2"/>
@@ -6745,17 +6788,17 @@
       <c r="D157" s="2"/>
       <c r="E157" s="9"/>
     </row>
-    <row r="233" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B233" s="2"/>
-      <c r="C233" s="2"/>
-      <c r="D233" s="2"/>
-      <c r="E233" s="9"/>
-    </row>
-    <row r="234" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B234" s="2"/>
-      <c r="C234" s="2"/>
-      <c r="D234" s="2"/>
-      <c r="E234" s="9"/>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="9"/>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="9"/>
     </row>
     <row r="235" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B235" s="2"/>
@@ -6893,6 +6936,7 @@
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
+      <c r="E257" s="9"/>
     </row>
     <row r="258" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B258" s="2"/>
@@ -6904,7 +6948,6 @@
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
-      <c r="E259" s="9"/>
     </row>
     <row r="260" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B260" s="2"/>
@@ -6936,28 +6979,30 @@
       <c r="D264" s="2"/>
       <c r="E264" s="9"/>
     </row>
-    <row r="947" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F947" s="2"/>
-    </row>
-    <row r="1083" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1083" s="2"/>
-      <c r="C1083" s="2"/>
-      <c r="D1083" s="2"/>
-    </row>
-    <row r="1084" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1084" s="2"/>
-      <c r="C1084" s="2"/>
-      <c r="D1084" s="2"/>
-    </row>
-    <row r="1209" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1209" s="2"/>
-      <c r="C1209" s="2"/>
-      <c r="D1209" s="2"/>
-    </row>
-    <row r="1210" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1210" s="2"/>
-      <c r="C1210" s="2"/>
-      <c r="D1210" s="2"/>
+    <row r="265" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B265" s="2"/>
+      <c r="C265" s="2"/>
+      <c r="D265" s="2"/>
+      <c r="E265" s="9"/>
+    </row>
+    <row r="266" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B266" s="2"/>
+      <c r="C266" s="2"/>
+      <c r="D266" s="2"/>
+      <c r="E266" s="9"/>
+    </row>
+    <row r="949" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F949" s="2"/>
+    </row>
+    <row r="1085" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1085" s="2"/>
+      <c r="C1085" s="2"/>
+      <c r="D1085" s="2"/>
+    </row>
+    <row r="1086" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1086" s="2"/>
+      <c r="C1086" s="2"/>
+      <c r="D1086" s="2"/>
     </row>
     <row r="1211" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1211" s="2"/>
@@ -6979,27 +7024,27 @@
       <c r="C1214" s="2"/>
       <c r="D1214" s="2"/>
     </row>
-    <row r="1259" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F1259" s="2"/>
-      <c r="G1259" s="2"/>
-    </row>
-    <row r="1260" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F1260" s="2"/>
-      <c r="G1260" s="2"/>
-    </row>
-    <row r="1261" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1215" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1215" s="2"/>
+      <c r="C1215" s="2"/>
+      <c r="D1215" s="2"/>
+    </row>
+    <row r="1216" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1216" s="2"/>
+      <c r="C1216" s="2"/>
+      <c r="D1216" s="2"/>
+    </row>
+    <row r="1261" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F1261" s="2"/>
       <c r="G1261" s="2"/>
     </row>
-    <row r="1263" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1263" s="2"/>
-      <c r="C1263" s="2"/>
-      <c r="D1263" s="2"/>
-    </row>
-    <row r="1264" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1264" s="2"/>
-      <c r="C1264" s="2"/>
-      <c r="D1264" s="2"/>
+    <row r="1262" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F1262" s="2"/>
+      <c r="G1262" s="2"/>
+    </row>
+    <row r="1263" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F1263" s="2"/>
+      <c r="G1263" s="2"/>
     </row>
     <row r="1265" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1265" s="2"/>
@@ -7016,15 +7061,15 @@
       <c r="C1267" s="2"/>
       <c r="D1267" s="2"/>
     </row>
-    <row r="1286" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1286" s="2"/>
-      <c r="C1286" s="2"/>
-      <c r="D1286" s="2"/>
-    </row>
-    <row r="1287" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1287" s="2"/>
-      <c r="C1287" s="2"/>
-      <c r="D1287" s="2"/>
+    <row r="1268" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1268" s="2"/>
+      <c r="C1268" s="2"/>
+      <c r="D1268" s="2"/>
+    </row>
+    <row r="1269" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1269" s="2"/>
+      <c r="C1269" s="2"/>
+      <c r="D1269" s="2"/>
     </row>
     <row r="1288" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1288" s="2"/>
@@ -7051,16 +7096,16 @@
       <c r="C1292" s="2"/>
       <c r="D1292" s="2"/>
     </row>
+    <row r="1293" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1293" s="2"/>
+      <c r="C1293" s="2"/>
+      <c r="D1293" s="2"/>
+    </row>
     <row r="1294" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1294" s="2"/>
       <c r="C1294" s="2"/>
       <c r="D1294" s="2"/>
     </row>
-    <row r="1295" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1295" s="2"/>
-      <c r="C1295" s="2"/>
-      <c r="D1295" s="2"/>
-    </row>
     <row r="1296" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1296" s="2"/>
       <c r="C1296" s="2"/>
@@ -7081,15 +7126,15 @@
       <c r="C1299" s="2"/>
       <c r="D1299" s="2"/>
     </row>
-    <row r="1351" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1351" s="2"/>
-      <c r="C1351" s="2"/>
-      <c r="D1351" s="2"/>
-    </row>
-    <row r="1352" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1352" s="2"/>
-      <c r="C1352" s="2"/>
-      <c r="D1352" s="2"/>
+    <row r="1300" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1300" s="2"/>
+      <c r="C1300" s="2"/>
+      <c r="D1300" s="2"/>
+    </row>
+    <row r="1301" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1301" s="2"/>
+      <c r="C1301" s="2"/>
+      <c r="D1301" s="2"/>
     </row>
     <row r="1353" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1353" s="2"/>
@@ -7101,16 +7146,16 @@
       <c r="C1354" s="2"/>
       <c r="D1354" s="2"/>
     </row>
+    <row r="1355" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1355" s="2"/>
+      <c r="C1355" s="2"/>
+      <c r="D1355" s="2"/>
+    </row>
     <row r="1356" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1356" s="2"/>
       <c r="C1356" s="2"/>
       <c r="D1356" s="2"/>
     </row>
-    <row r="1357" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1357" s="2"/>
-      <c r="C1357" s="2"/>
-      <c r="D1357" s="2"/>
-    </row>
     <row r="1358" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1358" s="2"/>
       <c r="C1358" s="2"/>
@@ -7121,15 +7166,15 @@
       <c r="C1359" s="2"/>
       <c r="D1359" s="2"/>
     </row>
-    <row r="1394" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1394" s="2"/>
-      <c r="C1394" s="2"/>
-      <c r="D1394" s="2"/>
-    </row>
-    <row r="1395" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1395" s="2"/>
-      <c r="C1395" s="2"/>
-      <c r="D1395" s="2"/>
+    <row r="1360" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1360" s="2"/>
+      <c r="C1360" s="2"/>
+      <c r="D1360" s="2"/>
+    </row>
+    <row r="1361" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1361" s="2"/>
+      <c r="C1361" s="2"/>
+      <c r="D1361" s="2"/>
     </row>
     <row r="1396" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1396" s="2"/>
@@ -7151,17 +7196,17 @@
       <c r="C1399" s="2"/>
       <c r="D1399" s="2"/>
     </row>
-    <row r="1441" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="F1441" s="2"/>
-      <c r="G1441" s="2"/>
-    </row>
-    <row r="1442" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E1442" s="10"/>
-      <c r="F1442" s="2"/>
-      <c r="G1442" s="2"/>
+    <row r="1400" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1400" s="2"/>
+      <c r="C1400" s="2"/>
+      <c r="D1400" s="2"/>
+    </row>
+    <row r="1401" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1401" s="2"/>
+      <c r="C1401" s="2"/>
+      <c r="D1401" s="2"/>
     </row>
     <row r="1443" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E1443" s="10"/>
       <c r="F1443" s="2"/>
       <c r="G1443" s="2"/>
     </row>
@@ -7171,18 +7216,18 @@
       <c r="G1444" s="2"/>
     </row>
     <row r="1445" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1445" s="10"/>
       <c r="F1445" s="2"/>
       <c r="G1445" s="2"/>
     </row>
-    <row r="1508" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1508" s="2"/>
-      <c r="C1508" s="2"/>
-      <c r="D1508" s="2"/>
-    </row>
-    <row r="1509" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1509" s="2"/>
-      <c r="C1509" s="2"/>
-      <c r="D1509" s="2"/>
+    <row r="1446" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1446" s="10"/>
+      <c r="F1446" s="2"/>
+      <c r="G1446" s="2"/>
+    </row>
+    <row r="1447" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F1447" s="2"/>
+      <c r="G1447" s="2"/>
     </row>
     <row r="1510" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1510" s="2"/>
@@ -7193,6 +7238,16 @@
       <c r="B1511" s="2"/>
       <c r="C1511" s="2"/>
       <c r="D1511" s="2"/>
+    </row>
+    <row r="1512" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1512" s="2"/>
+      <c r="C1512" s="2"/>
+      <c r="D1512" s="2"/>
+    </row>
+    <row r="1513" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1513" s="2"/>
+      <c r="C1513" s="2"/>
+      <c r="D1513" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G54">

</xml_diff>

<commit_message>
Added starling circovirus features
</commit_message>
<xml_diff>
--- a/tabular/core/reference_feature_locations.xlsx
+++ b/tabular/core/reference_feature_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8A2078-E77E-5C49-BE37-6EA626B03714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC92E315-B0C9-DC42-B698-D93084607851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26620" yWindow="1020" windowWidth="20860" windowHeight="24600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="97">
   <si>
     <t>featureName</t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>REF_Po-41</t>
-  </si>
-  <si>
-    <t>intergenic</t>
   </si>
   <si>
     <t>5UTR</t>
@@ -4928,10 +4925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1516"/>
+  <dimension ref="A1:G1515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="A1:G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4983,7 +4980,7 @@
         <v>45</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -5029,16 +5026,16 @@
         <v>45</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F4" s="6">
-        <v>994</v>
+        <v>1038</v>
       </c>
       <c r="G4" s="6">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
@@ -5052,36 +5049,36 @@
         <v>45</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="6">
-        <v>1038</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>8</v>
+        <v>1731</v>
+      </c>
+      <c r="G5" s="17">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="F6" s="6">
-        <v>1731</v>
-      </c>
-      <c r="G6" s="17">
-        <v>1758</v>
+        <v>108</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1007</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5098,13 +5095,13 @@
         <v>51</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="F7" s="6">
-        <v>108</v>
+        <v>550</v>
       </c>
       <c r="G7" s="6">
-        <v>1007</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5121,36 +5118,36 @@
         <v>51</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F8" s="6">
-        <v>550</v>
+        <v>1240</v>
       </c>
       <c r="G8" s="6">
-        <v>1026</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>20</v>
+      <c r="A9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F9" s="6">
-        <v>1240</v>
+        <v>32</v>
       </c>
       <c r="G9" s="6">
-        <v>1974</v>
+        <v>904</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -5167,36 +5164,36 @@
         <v>52</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F10" s="6">
-        <v>32</v>
+        <v>1154</v>
       </c>
       <c r="G10" s="6">
-        <v>904</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>22</v>
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F11" s="6">
-        <v>1154</v>
+        <v>51</v>
       </c>
       <c r="G11" s="6">
-        <v>1906</v>
+        <v>995</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -5213,13 +5210,13 @@
         <v>46</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="F12" s="6">
-        <v>51</v>
+        <v>357</v>
       </c>
       <c r="G12" s="6">
-        <v>995</v>
+        <v>671</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -5236,36 +5233,36 @@
         <v>46</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="F13" s="6">
-        <v>357</v>
+        <v>1034</v>
       </c>
       <c r="G13" s="6">
-        <v>671</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F14" s="6">
-        <v>1034</v>
+        <v>37</v>
       </c>
       <c r="G14" s="6">
-        <v>1735</v>
+        <v>906</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -5273,22 +5270,22 @@
         <v>23</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="F15" s="6">
-        <v>37</v>
+        <v>834</v>
       </c>
       <c r="G15" s="6">
-        <v>906</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -5296,45 +5293,45 @@
         <v>23</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F16" s="6">
-        <v>834</v>
+        <v>1190</v>
       </c>
       <c r="G16" s="6">
-        <v>1154</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>97</v>
+      <c r="A17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F17" s="6">
-        <v>1190</v>
+        <v>48</v>
       </c>
       <c r="G17" s="6">
-        <v>2020</v>
+        <v>926</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -5351,13 +5348,13 @@
         <v>57</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="F18" s="6">
-        <v>48</v>
+        <v>423</v>
       </c>
       <c r="G18" s="6">
-        <v>926</v>
+        <v>827</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -5374,36 +5371,36 @@
         <v>57</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F19" s="6">
-        <v>423</v>
+        <v>1155</v>
       </c>
       <c r="G19" s="6">
-        <v>827</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F20" s="6">
-        <v>1155</v>
+        <v>37</v>
       </c>
       <c r="G20" s="6">
-        <v>1928</v>
+        <v>906</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -5420,36 +5417,36 @@
         <v>53</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F21" s="6">
-        <v>37</v>
+        <v>1190</v>
       </c>
       <c r="G21" s="6">
-        <v>906</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F22" s="6">
-        <v>1190</v>
+        <v>36</v>
       </c>
       <c r="G22" s="6">
-        <v>2020</v>
+        <v>911</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -5459,43 +5456,43 @@
       <c r="B23" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F23" s="6">
-        <v>36</v>
+        <v>1116</v>
       </c>
       <c r="G23" s="6">
-        <v>911</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F24" s="6">
-        <v>1116</v>
+        <v>100</v>
       </c>
       <c r="G24" s="6">
-        <v>1844</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -5512,13 +5509,13 @@
         <v>55</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="F25" s="6">
-        <v>100</v>
+        <v>790</v>
       </c>
       <c r="G25" s="6">
-        <v>1017</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -5535,105 +5532,105 @@
         <v>55</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F26" s="6">
-        <v>790</v>
+        <v>1190</v>
       </c>
       <c r="G26" s="6">
-        <v>1209</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>27</v>
+      <c r="A27" t="s">
+        <v>89</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F27" s="6">
-        <v>1190</v>
+        <v>41</v>
       </c>
       <c r="G27" s="6">
-        <v>1927</v>
+        <v>994</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="F28" s="6">
-        <v>41</v>
+        <v>410</v>
       </c>
       <c r="G28" s="6">
-        <v>994</v>
+        <v>790</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F29" s="6">
-        <v>410</v>
+        <v>1166</v>
       </c>
       <c r="G29" s="6">
-        <v>790</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="14" t="s">
+      <c r="A30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F30" s="6">
-        <v>1166</v>
+        <v>29</v>
       </c>
       <c r="G30" s="6">
-        <v>1987</v>
+        <v>904</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -5643,43 +5640,43 @@
       <c r="B31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F31" s="6">
-        <v>29</v>
+        <v>614</v>
       </c>
       <c r="G31" s="6">
-        <v>904</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>30</v>
+      <c r="A32" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F32" s="6">
-        <v>614</v>
+        <v>48</v>
       </c>
       <c r="G32" s="6">
-        <v>1063</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -5696,36 +5693,36 @@
         <v>60</v>
       </c>
       <c r="E33" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="6">
+        <v>1261</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="6">
-        <v>48</v>
-      </c>
-      <c r="G33" s="6">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="F34" s="6">
-        <v>1261</v>
+        <v>1</v>
       </c>
       <c r="G34" s="6">
-        <v>1761</v>
+        <v>912</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -5735,43 +5732,43 @@
       <c r="B35" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>48</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F35" s="6">
-        <v>1</v>
+        <v>1116</v>
       </c>
       <c r="G35" s="6">
-        <v>912</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F36" s="6">
-        <v>1116</v>
+        <v>36</v>
       </c>
       <c r="G36" s="6">
-        <v>1928</v>
+        <v>929</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -5788,36 +5785,36 @@
         <v>49</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F37" s="6">
-        <v>36</v>
+        <v>1020</v>
       </c>
       <c r="G37" s="6">
-        <v>929</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F38" s="6">
-        <v>1020</v>
+        <v>251</v>
       </c>
       <c r="G38" s="6">
-        <v>1703</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -5827,43 +5824,43 @@
       <c r="B39" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F39" s="6">
-        <v>251</v>
+        <v>1251</v>
       </c>
       <c r="G39" s="6">
-        <v>1195</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F40" s="6">
-        <v>1251</v>
+        <v>48</v>
       </c>
       <c r="G40" s="6">
-        <v>1934</v>
+        <v>929</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -5880,36 +5877,36 @@
         <v>58</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F41" s="6">
-        <v>48</v>
+        <v>968</v>
       </c>
       <c r="G41" s="6">
-        <v>929</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F42" s="6">
-        <v>968</v>
+        <v>29</v>
       </c>
       <c r="G42" s="6">
-        <v>1723</v>
+        <v>904</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -5926,13 +5923,13 @@
         <v>59</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="F43" s="6">
-        <v>29</v>
+        <v>1233</v>
       </c>
       <c r="G43" s="6">
-        <v>904</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -5952,10 +5949,10 @@
         <v>80</v>
       </c>
       <c r="F44" s="6">
-        <v>1233</v>
+        <v>1289</v>
       </c>
       <c r="G44" s="6">
-        <v>1967</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -5972,36 +5969,36 @@
         <v>59</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F45" s="6">
-        <v>1289</v>
+        <v>1233</v>
       </c>
       <c r="G45" s="6">
-        <v>1720</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>36</v>
+      <c r="A46" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F46" s="6">
-        <v>1233</v>
+        <v>8</v>
       </c>
       <c r="G46" s="6">
-        <v>1772</v>
+        <v>919</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -6018,36 +6015,36 @@
         <v>50</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F47" s="6">
-        <v>8</v>
+        <v>1055</v>
       </c>
       <c r="G47" s="6">
-        <v>919</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F48" s="6">
-        <v>1055</v>
+        <v>216</v>
       </c>
       <c r="G48" s="6">
-        <v>1711</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -6064,36 +6061,36 @@
         <v>47</v>
       </c>
       <c r="E49" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" s="6">
+        <v>1336</v>
+      </c>
+      <c r="G49" s="6">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F49" s="6">
-        <v>216</v>
-      </c>
-      <c r="G49" s="6">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="F50" s="6">
-        <v>1336</v>
+        <v>26</v>
       </c>
       <c r="G50" s="6">
-        <v>1980</v>
+        <v>856</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -6110,36 +6107,36 @@
         <v>67</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F51" s="6">
-        <v>26</v>
+        <v>836</v>
       </c>
       <c r="G51" s="6">
-        <v>856</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F52" s="6">
-        <v>836</v>
+        <v>208</v>
       </c>
       <c r="G52" s="6">
-        <v>1528</v>
+        <v>867</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -6156,36 +6153,36 @@
         <v>68</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F53" s="6">
-        <v>208</v>
+        <v>1005</v>
       </c>
       <c r="G53" s="6">
-        <v>867</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="16" t="s">
         <v>73</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="F54" s="6">
-        <v>1005</v>
+        <v>606</v>
       </c>
       <c r="G54" s="6">
-        <v>1703</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -6202,13 +6199,13 @@
         <v>75</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="F55" s="6">
-        <v>606</v>
+        <v>1741</v>
       </c>
       <c r="G55" s="6">
-        <v>1583</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -6225,180 +6222,163 @@
         <v>75</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="F56" s="6">
-        <v>1741</v>
+        <v>2329</v>
       </c>
       <c r="G56" s="6">
-        <v>2313</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>73</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="F57" s="6">
-        <v>2329</v>
+        <v>1</v>
       </c>
       <c r="G57" s="6">
-        <v>2904</v>
+        <v>819</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>73</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E58" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F58" s="6">
+        <v>827</v>
+      </c>
+      <c r="G58" s="6">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F58" s="6">
-        <v>1</v>
-      </c>
-      <c r="G58" s="6">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="F59" s="6">
-        <v>827</v>
+        <v>68</v>
       </c>
       <c r="G59" s="6">
-        <v>1498</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" s="19" t="s">
+      <c r="D60" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="E60" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F60" s="6">
+        <v>1164</v>
+      </c>
+      <c r="G60" s="6">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>86</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="B61" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="6">
-        <v>68</v>
-      </c>
-      <c r="G60" s="6">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="15" t="s">
+      <c r="F61" s="6">
+        <v>79</v>
+      </c>
+      <c r="G61" s="6">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C61" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F61" s="6">
-        <v>1164</v>
-      </c>
-      <c r="G61" s="6">
-        <v>2060</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>87</v>
-      </c>
-      <c r="B62" s="18" t="s">
+      <c r="D62" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>89</v>
-      </c>
       <c r="E62" s="6" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F62" s="6">
-        <v>79</v>
+        <v>1139</v>
       </c>
       <c r="G62" s="6">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>87</v>
-      </c>
-      <c r="B63" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F63" s="6">
-        <v>1139</v>
-      </c>
-      <c r="G63" s="6">
         <v>2086</v>
       </c>
     </row>
-    <row r="70" spans="5:5" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E70" s="8"/>
-    </row>
-    <row r="76" spans="5:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="5:5" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="8"/>
+    </row>
+    <row r="75" spans="5:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="9"/>
+    </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -6452,6 +6432,7 @@
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="9"/>
+      <c r="G92" s="2"/>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B93" s="2"/>
@@ -6465,7 +6446,6 @@
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="9"/>
-      <c r="G94" s="2"/>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
@@ -6586,13 +6566,13 @@
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="9"/>
+      <c r="F114" s="1"/>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="9"/>
-      <c r="F115" s="1"/>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
@@ -6616,12 +6596,12 @@
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
-      <c r="E119" s="9"/>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
+      <c r="E120" s="9"/>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
@@ -6869,11 +6849,11 @@
       <c r="D161" s="2"/>
       <c r="E161" s="9"/>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
-      <c r="E162" s="9"/>
+    <row r="237" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B237" s="2"/>
+      <c r="C237" s="2"/>
+      <c r="D237" s="2"/>
+      <c r="E237" s="9"/>
     </row>
     <row r="238" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B238" s="2"/>
@@ -7017,12 +6997,12 @@
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
-      <c r="E261" s="9"/>
     </row>
     <row r="262" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
+      <c r="E262" s="9"/>
     </row>
     <row r="263" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B263" s="2"/>
@@ -7060,24 +7040,23 @@
       <c r="D268" s="2"/>
       <c r="E268" s="9"/>
     </row>
-    <row r="269" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B269" s="2"/>
-      <c r="C269" s="2"/>
-      <c r="D269" s="2"/>
-      <c r="E269" s="9"/>
-    </row>
-    <row r="952" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F952" s="2"/>
+    <row r="951" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F951" s="2"/>
+    </row>
+    <row r="1087" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1087" s="2"/>
+      <c r="C1087" s="2"/>
+      <c r="D1087" s="2"/>
     </row>
     <row r="1088" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1088" s="2"/>
       <c r="C1088" s="2"/>
       <c r="D1088" s="2"/>
     </row>
-    <row r="1089" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1089" s="2"/>
-      <c r="C1089" s="2"/>
-      <c r="D1089" s="2"/>
+    <row r="1213" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1213" s="2"/>
+      <c r="C1213" s="2"/>
+      <c r="D1213" s="2"/>
     </row>
     <row r="1214" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1214" s="2"/>
@@ -7104,10 +7083,9 @@
       <c r="C1218" s="2"/>
       <c r="D1218" s="2"/>
     </row>
-    <row r="1219" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1219" s="2"/>
-      <c r="C1219" s="2"/>
-      <c r="D1219" s="2"/>
+    <row r="1263" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F1263" s="2"/>
+      <c r="G1263" s="2"/>
     </row>
     <row r="1264" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F1264" s="2"/>
@@ -7117,9 +7095,10 @@
       <c r="F1265" s="2"/>
       <c r="G1265" s="2"/>
     </row>
-    <row r="1266" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F1266" s="2"/>
-      <c r="G1266" s="2"/>
+    <row r="1267" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1267" s="2"/>
+      <c r="C1267" s="2"/>
+      <c r="D1267" s="2"/>
     </row>
     <row r="1268" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1268" s="2"/>
@@ -7141,10 +7120,10 @@
       <c r="C1271" s="2"/>
       <c r="D1271" s="2"/>
     </row>
-    <row r="1272" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1272" s="2"/>
-      <c r="C1272" s="2"/>
-      <c r="D1272" s="2"/>
+    <row r="1290" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1290" s="2"/>
+      <c r="C1290" s="2"/>
+      <c r="D1290" s="2"/>
     </row>
     <row r="1291" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1291" s="2"/>
@@ -7176,10 +7155,10 @@
       <c r="C1296" s="2"/>
       <c r="D1296" s="2"/>
     </row>
-    <row r="1297" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1297" s="2"/>
-      <c r="C1297" s="2"/>
-      <c r="D1297" s="2"/>
+    <row r="1298" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1298" s="2"/>
+      <c r="C1298" s="2"/>
+      <c r="D1298" s="2"/>
     </row>
     <row r="1299" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1299" s="2"/>
@@ -7206,10 +7185,10 @@
       <c r="C1303" s="2"/>
       <c r="D1303" s="2"/>
     </row>
-    <row r="1304" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1304" s="2"/>
-      <c r="C1304" s="2"/>
-      <c r="D1304" s="2"/>
+    <row r="1355" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1355" s="2"/>
+      <c r="C1355" s="2"/>
+      <c r="D1355" s="2"/>
     </row>
     <row r="1356" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1356" s="2"/>
@@ -7226,10 +7205,10 @@
       <c r="C1358" s="2"/>
       <c r="D1358" s="2"/>
     </row>
-    <row r="1359" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1359" s="2"/>
-      <c r="C1359" s="2"/>
-      <c r="D1359" s="2"/>
+    <row r="1360" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1360" s="2"/>
+      <c r="C1360" s="2"/>
+      <c r="D1360" s="2"/>
     </row>
     <row r="1361" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1361" s="2"/>
@@ -7246,10 +7225,10 @@
       <c r="C1363" s="2"/>
       <c r="D1363" s="2"/>
     </row>
-    <row r="1364" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1364" s="2"/>
-      <c r="C1364" s="2"/>
-      <c r="D1364" s="2"/>
+    <row r="1398" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1398" s="2"/>
+      <c r="C1398" s="2"/>
+      <c r="D1398" s="2"/>
     </row>
     <row r="1399" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1399" s="2"/>
@@ -7276,12 +7255,12 @@
       <c r="C1403" s="2"/>
       <c r="D1403" s="2"/>
     </row>
-    <row r="1404" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1404" s="2"/>
-      <c r="C1404" s="2"/>
-      <c r="D1404" s="2"/>
+    <row r="1445" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F1445" s="2"/>
+      <c r="G1445" s="2"/>
     </row>
     <row r="1446" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1446" s="10"/>
       <c r="F1446" s="2"/>
       <c r="G1446" s="2"/>
     </row>
@@ -7296,13 +7275,13 @@
       <c r="G1448" s="2"/>
     </row>
     <row r="1449" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E1449" s="10"/>
       <c r="F1449" s="2"/>
       <c r="G1449" s="2"/>
     </row>
-    <row r="1450" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="F1450" s="2"/>
-      <c r="G1450" s="2"/>
+    <row r="1512" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1512" s="2"/>
+      <c r="C1512" s="2"/>
+      <c r="D1512" s="2"/>
     </row>
     <row r="1513" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1513" s="2"/>
@@ -7319,16 +7298,11 @@
       <c r="C1515" s="2"/>
       <c r="D1515" s="2"/>
     </row>
-    <row r="1516" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1516" s="2"/>
-      <c r="C1516" s="2"/>
-      <c r="D1516" s="2"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G57">
-    <sortCondition ref="C3:C57"/>
-    <sortCondition ref="A3:A57"/>
-    <sortCondition ref="F3:F57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G56">
+    <sortCondition ref="C3:C56"/>
+    <sortCondition ref="A3:A56"/>
+    <sortCondition ref="F3:F56"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Refactoring - putting all cyclocviruses in same orientation
</commit_message>
<xml_diff>
--- a/tabular/core/reference_feature_locations.xlsx
+++ b/tabular/core/reference_feature_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EA73FD-308F-0348-9929-1A9717762055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A463C9-077A-D941-8CEA-605DB463FFFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="460" windowWidth="26220" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,9 +319,6 @@
     <t>REF_Cyclo_MASTER_HuACyV-1</t>
   </si>
   <si>
-    <t>REF_CRESS1_MASTER_Po-41</t>
-  </si>
-  <si>
     <t>whole_genome</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>CBSV</t>
+  </si>
+  <si>
+    <t>REF_CRESS2_MASTER_Po-41</t>
   </si>
 </sst>
 </file>
@@ -4974,8 +4974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1540"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D85" sqref="A1:G91"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5027,7 +5027,7 @@
         <v>72</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -5142,7 +5142,7 @@
         <v>73</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F7" s="6">
         <v>1</v>
@@ -5234,7 +5234,7 @@
         <v>74</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F11" s="6">
         <v>1</v>
@@ -5303,7 +5303,7 @@
         <v>75</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F14" s="6">
         <v>1</v>
@@ -5395,7 +5395,7 @@
         <v>76</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F18" s="6">
         <v>1</v>
@@ -5487,7 +5487,7 @@
         <v>77</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F22" s="6">
         <v>1</v>
@@ -5579,7 +5579,7 @@
         <v>78</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="6">
         <v>1</v>
@@ -5648,7 +5648,7 @@
         <v>79</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F29" s="6">
         <v>1</v>
@@ -5717,7 +5717,7 @@
         <v>80</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F32" s="6">
         <v>1</v>
@@ -5809,7 +5809,7 @@
         <v>81</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F36" s="6">
         <v>1</v>
@@ -5901,7 +5901,7 @@
         <v>82</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F40" s="6">
         <v>1</v>
@@ -5970,7 +5970,7 @@
         <v>83</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F43" s="6">
         <v>1</v>
@@ -6039,7 +6039,7 @@
         <v>84</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F46" s="6">
         <v>1</v>
@@ -6108,7 +6108,7 @@
         <v>85</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F49" s="6">
         <v>1</v>
@@ -6177,7 +6177,7 @@
         <v>86</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F52" s="6">
         <v>1</v>
@@ -6246,7 +6246,7 @@
         <v>87</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F55" s="6">
         <v>1</v>
@@ -6315,7 +6315,7 @@
         <v>88</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F58" s="6">
         <v>1</v>
@@ -6430,7 +6430,7 @@
         <v>89</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F63" s="6">
         <v>1</v>
@@ -6499,7 +6499,7 @@
         <v>90</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F66" s="6">
         <v>1</v>
@@ -6568,7 +6568,7 @@
         <v>95</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F69" s="6">
         <v>1</v>
@@ -6637,7 +6637,7 @@
         <v>91</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F72" s="6">
         <v>1</v>
@@ -6703,10 +6703,10 @@
         <v>54</v>
       </c>
       <c r="D75" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="F75" s="6">
         <v>1</v>
@@ -6726,7 +6726,7 @@
         <v>54</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>41</v>
@@ -6749,7 +6749,7 @@
         <v>54</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>45</v>
@@ -6772,7 +6772,7 @@
         <v>54</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>61</v>
@@ -6798,7 +6798,7 @@
         <v>92</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F79" s="6">
         <v>1</v>
@@ -6867,7 +6867,7 @@
         <v>93</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F82" s="6">
         <v>1</v>
@@ -6892,11 +6892,11 @@
       <c r="E83" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F83" s="6">
-        <v>68</v>
-      </c>
-      <c r="G83" s="6">
-        <v>1171</v>
+      <c r="F83">
+        <v>153</v>
+      </c>
+      <c r="G83">
+        <v>1049</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -6915,11 +6915,11 @@
       <c r="E84" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F84" s="6">
-        <v>1164</v>
-      </c>
-      <c r="G84" s="6">
-        <v>2060</v>
+      <c r="F84">
+        <v>1042</v>
+      </c>
+      <c r="G84">
+        <v>2145</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -6936,7 +6936,7 @@
         <v>94</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F85" s="6">
         <v>1</v>
@@ -6993,19 +6993,19 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C88" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F88" s="6">
         <v>1</v>
@@ -7016,16 +7016,16 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C89" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>41</v>
@@ -7039,16 +7039,16 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C90" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>50</v>
@@ -7062,16 +7062,16 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C91" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Refactoring - set up core project with master references only
</commit_message>
<xml_diff>
--- a/tabular/core/reference_feature_locations.xlsx
+++ b/tabular/core/reference_feature_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A463C9-077A-D941-8CEA-605DB463FFFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3C960A-82A7-B44F-9E0D-D2E618B2D136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="26220" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="26220" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4974,8 +4974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1540"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69:G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>